<commit_message>
plan de projet v0.8
v0.8
</commit_message>
<xml_diff>
--- a/Plan_de_projet.xlsx
+++ b/Plan_de_projet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\BabyRoger\Desktop\projet_2ieme_annee\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\wamp64\www\Projet2A\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="2" r:id="rId1"/>
@@ -28,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
-  <si>
-    <t xml:space="preserve">Description Technique : </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="52">
   <si>
     <t>Utilisation du framework Symphony 3 pour l'application de gestion ET l'application client</t>
   </si>
@@ -114,9 +111,6 @@
     <t>Visualisation d'anciens abonnements</t>
   </si>
   <si>
-    <t>Système d'authetification par challenge/reponse</t>
-  </si>
-  <si>
     <t>Economiser la data utilisateur</t>
   </si>
   <si>
@@ -133,13 +127,77 @@
   </si>
   <si>
     <t>LIVRAISON LE 6 JUILLET</t>
+  </si>
+  <si>
+    <t>CRUD Utilisateur</t>
+  </si>
+  <si>
+    <t>CRUD Abonnement</t>
+  </si>
+  <si>
+    <t>CRUD Paiement</t>
+  </si>
+  <si>
+    <t>CRUD Magasine</t>
+  </si>
+  <si>
+    <t>CRUD Historique</t>
+  </si>
+  <si>
+    <t>Authentification (challenge/reponse)</t>
+  </si>
+  <si>
+    <t>Système d'authentification par challenge/reponse</t>
+  </si>
+  <si>
+    <t>Mise en place serveur Mail</t>
+  </si>
+  <si>
+    <t>Création d'un CRON Quotidien</t>
+  </si>
+  <si>
+    <t>Traitement statistique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Création de compte   </t>
+  </si>
+  <si>
+    <t>Optimisation</t>
+  </si>
+  <si>
+    <t>FONCTIONNALITE</t>
+  </si>
+  <si>
+    <t>EXIGENCE</t>
+  </si>
+  <si>
+    <t>Authentification</t>
+  </si>
+  <si>
+    <t>JALON 1   =&gt; 16/06</t>
+  </si>
+  <si>
+    <t>JALON 4</t>
+  </si>
+  <si>
+    <t>JALON 2 =&gt; 21/06</t>
+  </si>
+  <si>
+    <t>JALON 3 =&gt; 26/06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,7 +214,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -164,12 +222,124 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,12 +664,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -509,177 +679,177 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection sqref="A1:F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>19</v>
+      <c r="B18" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>30</v>
+      <c r="C29" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>32</v>
+      <c r="B31" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>34</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -689,29 +859,238 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:A22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.42578125" customWidth="1"/>
+    <col min="2" max="2" width="53" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -721,12 +1100,90 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>